<commit_message>
error hanlle in login
</commit_message>
<xml_diff>
--- a/Blog/server/data.xlsx
+++ b/Blog/server/data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,6 +415,21 @@
       <c r="D1" t="str">
         <v>author</v>
       </c>
+      <c r="E1" t="str">
+        <v>0</v>
+      </c>
+      <c r="F1" t="str">
+        <v>1</v>
+      </c>
+      <c r="G1" t="str">
+        <v>2</v>
+      </c>
+      <c r="H1" t="str">
+        <v>3</v>
+      </c>
+      <c r="I1" t="str">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" xml:space="preserve">
       <c r="A2">
@@ -464,9 +479,10 @@
         <v>1733119848750</v>
       </c>
     </row>
+    <row r="6"/>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:I6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>